<commit_message>
rename variables for consistency with standard.
</commit_message>
<xml_diff>
--- a/utilityscripts/earthquake/as1170_4_data.xlsx
+++ b/utilityscripts/earthquake/as1170_4_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sean Kane\PycharmProjects\utilityscripts\utilityscripts\earthquake\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FE4994E-7E12-43BA-8CC4-4A9DE15B64FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D7E1FB-5D0F-486E-827A-AD74705C1DEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-270" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="soil_descriptors" sheetId="2" r:id="rId1"/>
@@ -37,10 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
-  <si>
-    <t>soil_type</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="19">
   <si>
     <t>min_period</t>
   </si>
@@ -78,9 +75,6 @@
     <t>Ee</t>
   </si>
   <si>
-    <t>class</t>
-  </si>
-  <si>
     <t>description</t>
   </si>
   <si>
@@ -97,6 +91,9 @@
   </si>
   <si>
     <t>Very Soft Soil</t>
+  </si>
+  <si>
+    <t>soil_class</t>
   </si>
 </sst>
 </file>
@@ -421,8 +418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A89FF0C-7770-477B-B4CF-604A6C2AC458}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -432,50 +429,50 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -487,8 +484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,33 +497,33 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
       <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" t="s">
-        <v>8</v>
-      </c>
       <c r="H1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -553,7 +550,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>0.1</v>
@@ -579,7 +576,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>1.5</v>
@@ -605,7 +602,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -631,7 +628,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>0.1</v>
@@ -657,7 +654,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7">
         <v>1.5</v>
@@ -683,7 +680,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -709,7 +706,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9">
         <v>0.1</v>
@@ -735,7 +732,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>1.5</v>
@@ -761,7 +758,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -787,7 +784,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>0.1</v>
@@ -813,7 +810,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13">
         <v>1.5</v>
@@ -839,7 +836,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -865,7 +862,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B15">
         <v>0.1</v>
@@ -891,7 +888,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B16">
         <v>1.5</v>

</xml_diff>

<commit_message>
add k_p method, update tests.
</commit_message>
<xml_diff>
--- a/utilityscripts/earthquake/as1170_4_data.xlsx
+++ b/utilityscripts/earthquake/as1170_4_data.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sean Kane\PycharmProjects\utilityscripts\utilityscripts\earthquake\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D7E1FB-5D0F-486E-827A-AD74705C1DEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A14A379E-3187-4CB3-81DB-09DDC1370C39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-270" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-270" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="soil_descriptors" sheetId="2" r:id="rId1"/>
     <sheet name="soil_spectra" sheetId="1" r:id="rId2"/>
+    <sheet name="k_p" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
   <si>
     <t>min_period</t>
   </si>
@@ -94,6 +95,12 @@
   </si>
   <si>
     <t>soil_class</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>k_p</t>
   </si>
 </sst>
 </file>
@@ -418,7 +425,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A89FF0C-7770-477B-B4CF-604A6C2AC458}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -915,4 +922,99 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D5F6D89-B544-4EED-BEFC-AE081B6C778A}">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2500</v>
+      </c>
+      <c r="B2">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2000</v>
+      </c>
+      <c r="B3">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1500</v>
+      </c>
+      <c r="B4">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1000</v>
+      </c>
+      <c r="B5">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>800</v>
+      </c>
+      <c r="B6">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>500</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>250</v>
+      </c>
+      <c r="B8">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>200</v>
+      </c>
+      <c r="B9">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>100</v>
+      </c>
+      <c r="B10">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
as1170_4 add kp_z_min method and update C_dt to use the values from it.
</commit_message>
<xml_diff>
--- a/utilityscripts/earthquake/as1170_4_data.xlsx
+++ b/utilityscripts/earthquake/as1170_4_data.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sean Kane\PycharmProjects\utilityscripts\utilityscripts\earthquake\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A14A379E-3187-4CB3-81DB-09DDC1370C39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C8E497A-F81D-41DA-B811-FE2A34481EFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-270" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="soil_descriptors" sheetId="2" r:id="rId1"/>
     <sheet name="soil_spectra" sheetId="1" r:id="rId2"/>
     <sheet name="k_p" sheetId="3" r:id="rId3"/>
+    <sheet name="k_p_z_min" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="22">
   <si>
     <t>min_period</t>
   </si>
@@ -101,6 +102,9 @@
   </si>
   <si>
     <t>k_p</t>
+  </si>
+  <si>
+    <t>k_p_z_min</t>
   </si>
 </sst>
 </file>
@@ -928,7 +932,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D5F6D89-B544-4EED-BEFC-AE081B6C778A}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -1017,4 +1021,67 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24A36A5C-1DDA-4BB9-8121-49222B011D9A}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>500</v>
+      </c>
+      <c r="B2">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1000</v>
+      </c>
+      <c r="B3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1500</v>
+      </c>
+      <c r="B4">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2000</v>
+      </c>
+      <c r="B5">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2500</v>
+      </c>
+      <c r="B6">
+        <v>0.15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>